<commit_message>
added new import template
</commit_message>
<xml_diff>
--- a/src/assets/Import_Vorlage.xlsx
+++ b/src/assets/Import_Vorlage.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E6ABC7-8884-4928-A229-D6B3E95022CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD26FB4F-F1DA-43A6-B5D5-55223251EE22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28755" yWindow="270" windowWidth="25200" windowHeight="16335" xr2:uid="{1F47A2D3-FB1C-43B3-B4EE-680EF7A940FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{1F47A2D3-FB1C-43B3-B4EE-680EF7A940FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Struktur-Vorschlag" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{BC854CA5-9EA5-4FFC-A278-5E1771508DAF}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B6B490A6-6743-4B39-A526-A91A5D5F520F}">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{EAB89E7C-61B0-44C7-93C6-3E2EBDB7A484}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{F96C741E-9EE6-4E7C-AD68-5330654019E9}">
       <text>
         <r>
           <rPr>
@@ -83,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{3FC767A6-6756-4594-85F4-62042AEEDCE2}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{CAEE28E7-66CD-4633-BC82-3DE6573A12DB}">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{6F30EECF-F9C0-43D7-A6FD-00D6E5D9E8DD}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{A9BC2303-DE9C-4A1B-B21F-CBACCA1D2B5D}">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{D7A118E2-ADDD-4C7E-B2A3-1D9F83167C67}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{D9552E7E-BC67-4018-ACC3-DD0F3FF77E73}">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{E70DCFB0-F411-4D25-A5FC-6341E55154F6}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{ADAA50D8-3826-4082-857C-E4D8A5663D83}">
       <text>
         <r>
           <rPr>
@@ -171,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{DF3303AC-2405-48CC-8D18-FF1739D9C582}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{25B49421-70D5-481C-AF41-4B44A0787069}">
       <text>
         <r>
           <rPr>
@@ -195,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{133005DB-5BBD-4F98-B382-CA4D40964179}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{3C27026A-4400-4E0E-A0DE-9C698ABE0926}">
       <text>
         <r>
           <rPr>
@@ -219,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{5C0E1E82-33F5-4B18-AC62-F961B9EA5569}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{3BC7B0B9-F5FC-4D79-84B7-CA5ED5F9DC07}">
       <text>
         <r>
           <rPr>
@@ -243,7 +243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T5" authorId="0" shapeId="0" xr:uid="{A740CCD1-1162-465B-9F3D-1A9FA3595FA1}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{0B8D57F9-E841-4B21-AA15-CDA264E47B15}">
       <text>
         <r>
           <rPr>
@@ -267,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{B65B5F1A-8075-464A-930F-CFCB76D3541B}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{10C76DEA-4455-4BAF-B449-24E67AFA46D3}">
       <text>
         <r>
           <rPr>
@@ -296,15 +296,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
-  <si>
-    <t>ANLAGE 5 - LISTE DER BETREIBER VON TESTSTELLEN</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">NR. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LADUNGSFÄHIGE ANSCHRIFT </t>
   </si>
   <si>
     <t>ENTRITTSDATUM</t>
@@ -425,10 +419,6 @@
     <t>Thüringen</t>
   </si>
   <si>
-    <t>NAME/FIRMA DES BETREIBERS
-Vetragspartner</t>
-  </si>
-  <si>
     <t>Name Ansprechpartner/in</t>
   </si>
   <si>
@@ -444,9 +434,6 @@
     <t>Terminbuchung: [erforderlich, möglich, nicht notwendig]</t>
   </si>
   <si>
-    <t>Ausstellung eines Dicital Covid Zertifikates (DCC)</t>
-  </si>
-  <si>
     <t>Freitext</t>
   </si>
   <si>
@@ -460,13 +447,31 @@
   </si>
   <si>
     <t>Mo-Fr: 7 -18 Uhr|Sa: 7-12 Uhr</t>
+  </si>
+  <si>
+    <t>Sichtbar (Ja/Nein)</t>
+  </si>
+  <si>
+    <t>Ausstellung eines Dicital Covid Zertifikates (DCC) (Ja/Nein)</t>
+  </si>
+  <si>
+    <t>Name der Teststelle</t>
+  </si>
+  <si>
+    <t>Anschrift der Teststelle</t>
+  </si>
+  <si>
+    <t>Name des Betreibers</t>
+  </si>
+  <si>
+    <t>Lab ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,14 +482,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -504,7 +501,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,6 +520,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -622,42 +625,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -670,6 +645,32 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -679,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -690,23 +691,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -714,35 +727,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1058,148 +1062,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5810139C-4D50-4112-A85F-77014E68DEA4}">
-  <dimension ref="B3:T6"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="72.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="65" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" customWidth="1"/>
+    <col min="12" max="12" width="31.7109375" customWidth="1"/>
     <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.42578125" customWidth="1"/>
     <col min="15" max="15" width="18" customWidth="1"/>
     <col min="16" max="17" width="28.85546875" customWidth="1"/>
     <col min="18" max="18" width="64.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="28.85546875" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C3" s="9" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="C1" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="L1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="17" t="s">
+      <c r="P1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="P5" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q5" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="R5" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="S5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="T5" s="18" t="s">
+      <c r="J2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="C3:K3"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
+  <mergeCells count="17">
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1219,130 +1225,130 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed new import template
</commit_message>
<xml_diff>
--- a/src/assets/Import_Vorlage.xlsx
+++ b/src/assets/Import_Vorlage.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465308BC-D190-4716-BC46-636FB0DBF4C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BC7881-00BD-4796-98AD-D6123D56F7F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{1F47A2D3-FB1C-43B3-B4EE-680EF7A940FB}"/>
+    <workbookView xWindow="3480" yWindow="3315" windowWidth="21600" windowHeight="12615" xr2:uid="{1F47A2D3-FB1C-43B3-B4EE-680EF7A940FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Struktur-Vorschlag" sheetId="2" r:id="rId1"/>
@@ -272,7 +272,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">NR. </t>
   </si>
@@ -451,53 +451,17 @@
     <t>(Ja/Nein)</t>
   </si>
   <si>
-    <t>Betreiber</t>
-  </si>
-  <si>
-    <t>Teststelle</t>
-  </si>
-  <si>
-    <t>LabId</t>
-  </si>
-  <si>
-    <t>Burgker Str.</t>
-  </si>
-  <si>
-    <t>Freital</t>
-  </si>
-  <si>
-    <t>dirk.reske@gmx.net</t>
-  </si>
-  <si>
-    <t>Immer</t>
-  </si>
-  <si>
-    <t>möglich</t>
-  </si>
-  <si>
-    <t>Impfung</t>
-  </si>
-  <si>
-    <t>http://www.google.de</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
     <t>Adresshinweis</t>
   </si>
   <si>
     <t>z.B. Rollstuhlgerecht, Zugang</t>
-  </si>
-  <si>
-    <t>Zugang über Parkhaus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,14 +489,6 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -711,11 +667,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -756,10 +711,31 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -768,38 +744,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1112,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5810139C-4D50-4112-A85F-77014E68DEA4}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+      <selection activeCell="L3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,41 +1097,41 @@
       <c r="A1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="23" t="s">
         <v>39</v>
       </c>
       <c r="Q1" s="7" t="s">
@@ -1197,16 +1149,16 @@
       <c r="U1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="25" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1223,13 +1175,13 @@
         <v>3</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
+        <v>60</v>
+      </c>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
       <c r="Q2" s="5" t="s">
         <v>43</v>
       </c>
@@ -1245,86 +1197,26 @@
       <c r="U2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="V2" s="15"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="1">
-        <v>145</v>
-      </c>
-      <c r="H3">
-        <v>1705</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" t="s">
-        <v>72</v>
-      </c>
-      <c r="L3" s="28">
-        <v>44562</v>
-      </c>
-      <c r="M3" s="28">
-        <v>44926</v>
-      </c>
-      <c r="P3" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>65</v>
-      </c>
-      <c r="R3" t="s">
-        <v>66</v>
-      </c>
-      <c r="S3" t="s">
-        <v>67</v>
-      </c>
-      <c r="T3" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="U3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V3" t="s">
-        <v>69</v>
-      </c>
+      <c r="V2" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="P1:P2"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="P3" r:id="rId1" xr:uid="{19786C66-89ED-4122-85DC-394FF0E8B5BE}"/>
-    <hyperlink ref="T3" r:id="rId2" xr:uid="{FAE35F12-1CFF-4453-95B7-FF969BDF2738}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>